<commit_message>
small updates and bug fixes
</commit_message>
<xml_diff>
--- a/virome_abundance_meta_analysis/final_aggregate_tables/liang_stepwise_2020_phanta_aggregated.xlsx
+++ b/virome_abundance_meta_analysis/final_aggregate_tables/liang_stepwise_2020_phanta_aggregated.xlsx
@@ -13,7 +13,175 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="280">
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_345</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_340</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_333</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_398</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_395</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_394</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_396</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_395</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_398</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_428</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_400</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_401</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_389</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_385</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_376</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_352</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_357</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_359</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_365</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_375</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_373</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_365</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_368</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_345</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_subject_333</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>infant_month_1</t>
+  </si>
+  <si>
+    <t>infant_month_4</t>
+  </si>
+  <si>
+    <t>n_sample</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>liang_stepwise_2020_phanta</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>meta_bulk</t>
+  </si>
+  <si>
+    <t>mean_phage_load</t>
+  </si>
+  <si>
+    <t>sttdev_phage_load</t>
+  </si>
   <si>
     <t>subject</t>
   </si>
@@ -744,42 +912,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>194</v>
+        <v>250</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>217</v>
+        <v>273</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>218</v>
+        <v>274</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>220</v>
+        <v>276</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>222</v>
+        <v>278</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>223</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C2" s="0">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F2" s="0">
         <v>4704318345379.457</v>
@@ -788,19 +956,19 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F3" s="0">
         <v>366018434454.48199</v>
@@ -809,19 +977,19 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C4" s="0">
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F4" s="0">
         <v>266576979920.25616</v>
@@ -830,19 +998,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C5" s="0">
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F5" s="0">
         <v>632164807336.30334</v>
@@ -851,19 +1019,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>172</v>
+        <v>228</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C6" s="0">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F6" s="0">
         <v>421254327612.76648</v>
@@ -872,19 +1040,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>173</v>
+        <v>229</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C7" s="0">
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F7" s="0">
         <v>446372116954.41315</v>
@@ -893,19 +1061,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="C8" s="0">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F8" s="0">
         <v>150144436917.39941</v>
@@ -914,19 +1082,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>198</v>
+        <v>254</v>
       </c>
       <c r="C9" s="0">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F9" s="0">
         <v>667980144986.68689</v>
@@ -935,19 +1103,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>175</v>
+        <v>231</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>199</v>
+        <v>255</v>
       </c>
       <c r="C10" s="0">
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F10" s="0">
         <v>90381670301.854172</v>
@@ -956,19 +1124,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>175</v>
+        <v>231</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="C11" s="0">
         <v>1</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F11" s="0">
         <v>538520134264.42017</v>
@@ -977,19 +1145,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>176</v>
+        <v>232</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="C12" s="0">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F12" s="0">
         <v>404123367036.1134</v>
@@ -998,19 +1166,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>177</v>
+        <v>233</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="C13" s="0">
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F13" s="0">
         <v>419079872831.41315</v>
@@ -1019,19 +1187,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>178</v>
+        <v>234</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>200</v>
+        <v>256</v>
       </c>
       <c r="C14" s="0">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F14" s="0">
         <v>1124164130960.8896</v>
@@ -1040,19 +1208,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>178</v>
+        <v>234</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="C15" s="0">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F15" s="0">
         <v>531993764896.56122</v>
@@ -1061,19 +1229,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="C16" s="0">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F16" s="0">
         <v>444796975606.97375</v>
@@ -1082,19 +1250,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="C17" s="0">
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F17" s="0">
         <v>396692765364.60522</v>
@@ -1103,19 +1271,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="C18" s="0">
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F18" s="0">
         <v>420263568116.6236</v>
@@ -1124,19 +1292,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>202</v>
+        <v>258</v>
       </c>
       <c r="C19" s="0">
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F19" s="0">
         <v>332768095935.86383</v>
@@ -1145,19 +1313,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="C20" s="0">
         <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F20" s="0">
         <v>350899139338.60571</v>
@@ -1166,19 +1334,19 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="C21" s="0">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F21" s="0">
         <v>578963636842.24792</v>
@@ -1187,19 +1355,19 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>182</v>
+        <v>238</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="C22" s="0">
         <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F22" s="0">
         <v>227752478369.8266</v>
@@ -1208,19 +1376,19 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>204</v>
+        <v>260</v>
       </c>
       <c r="C23" s="0">
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F23" s="0">
         <v>248008689515.01309</v>
@@ -1229,19 +1397,19 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>183</v>
+        <v>239</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="C24" s="0">
         <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F24" s="0">
         <v>609302119262.3197</v>
@@ -1250,19 +1418,19 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>184</v>
+        <v>240</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="C25" s="0">
         <v>1</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F25" s="0">
         <v>370305754569.92529</v>
@@ -1271,19 +1439,19 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>184</v>
+        <v>240</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
       <c r="C26" s="0">
         <v>1</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F26" s="0">
         <v>427813201041.86469</v>
@@ -1292,19 +1460,19 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>185</v>
+        <v>241</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>207</v>
+        <v>263</v>
       </c>
       <c r="C27" s="0">
         <v>1</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F27" s="0">
         <v>94044290383.99913</v>
@@ -1313,19 +1481,19 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>185</v>
+        <v>241</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>208</v>
+        <v>264</v>
       </c>
       <c r="C28" s="0">
         <v>1</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F28" s="0">
         <v>219895626260.14383</v>
@@ -1334,19 +1502,19 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="C29" s="0">
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F29" s="0">
         <v>357601910899.74146</v>
@@ -1355,19 +1523,19 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="C30" s="0">
         <v>1</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F30" s="0">
         <v>534389009143.23547</v>
@@ -1376,19 +1544,19 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>187</v>
+        <v>243</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>211</v>
+        <v>267</v>
       </c>
       <c r="C31" s="0">
         <v>1</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F31" s="0">
         <v>403705420925.78387</v>
@@ -1397,19 +1565,19 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
       <c r="C32" s="0">
         <v>1</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F32" s="0">
         <v>420970794549.65857</v>
@@ -1418,19 +1586,19 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>188</v>
+        <v>244</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="C33" s="0">
         <v>1</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F33" s="0">
         <v>285077534465.82629</v>
@@ -1439,19 +1607,19 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="C34" s="0">
         <v>1</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F34" s="0">
         <v>178566643464.32651</v>
@@ -1460,19 +1628,19 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>189</v>
+        <v>245</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="C35" s="0">
         <v>1</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F35" s="0">
         <v>341056853610.91541</v>
@@ -1481,19 +1649,19 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>190</v>
+        <v>246</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="C36" s="0">
         <v>1</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F36" s="0">
         <v>496317985049.82501</v>
@@ -1502,19 +1670,19 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="C37" s="0">
         <v>1</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F37" s="0">
         <v>129716972270.08412</v>
@@ -1523,19 +1691,19 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>215</v>
+        <v>271</v>
       </c>
       <c r="C38" s="0">
         <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F38" s="0">
         <v>458593335037.18402</v>
@@ -1544,19 +1712,19 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>192</v>
+        <v>248</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="C39" s="0">
         <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F39" s="0">
         <v>226056513979.18015</v>
@@ -1565,19 +1733,19 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>193</v>
+        <v>249</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="C40" s="0">
         <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>219</v>
+        <v>275</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="F40" s="0">
         <v>282132785703.42419</v>

</xml_diff>